<commit_message>
sept 5, 2025 code
(the inclusion of bfm option in 06a was made on sept 16th)
</commit_message>
<xml_diff>
--- a/input_data/admin_data/ECU/_clean/total-pos-ECU.xlsx
+++ b/input_data/admin_data/ECU/_clean/total-pos-ECU.xlsx
@@ -16,7 +16,1855 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="1056">
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
   <si>
     <t>year</t>
   </si>
@@ -1386,22 +3234,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>352</v>
+        <v>968</v>
       </c>
       <c r="B1" t="s">
-        <v>353</v>
+        <v>969</v>
       </c>
       <c r="C1" t="s">
-        <v>362</v>
+        <v>978</v>
       </c>
       <c r="D1" t="s">
-        <v>363</v>
+        <v>979</v>
       </c>
       <c r="E1" t="s">
-        <v>364</v>
+        <v>980</v>
       </c>
       <c r="F1" t="s">
-        <v>373</v>
+        <v>989</v>
       </c>
     </row>
     <row r="2">
@@ -1409,7 +3257,7 @@
         <v>2008</v>
       </c>
       <c r="B2" t="s">
-        <v>354</v>
+        <v>970</v>
       </c>
       <c r="C2" s="1">
         <v>2821.7672837582504</v>
@@ -1418,7 +3266,7 @@
         <v>0.94089829921722412</v>
       </c>
       <c r="E2" t="s">
-        <v>365</v>
+        <v>981</v>
       </c>
       <c r="F2" s="1">
         <v>6201.1068160713085</v>
@@ -1427,14 +3275,14 @@
     <row r="3">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
-        <v>355</v>
+        <v>971</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1">
         <v>0.97042548656463623</v>
       </c>
       <c r="E3" t="s">
-        <v>366</v>
+        <v>982</v>
       </c>
       <c r="F3" s="1">
         <v>11701.011533552277</v>
@@ -1443,14 +3291,14 @@
     <row r="4">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
-        <v>356</v>
+        <v>972</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1">
         <v>0.99404728412628174</v>
       </c>
       <c r="E4" t="s">
-        <v>367</v>
+        <v>983</v>
       </c>
       <c r="F4" s="1">
         <v>34409.242584</v>
@@ -1459,14 +3307,14 @@
     <row r="5">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
-        <v>357</v>
+        <v>973</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1">
         <v>0.99700003862380981</v>
       </c>
       <c r="E5" t="s">
-        <v>368</v>
+        <v>984</v>
       </c>
       <c r="F5" s="1">
         <v>44915.427675000006</v>
@@ -1475,14 +3323,14 @@
     <row r="6">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
-        <v>358</v>
+        <v>974</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1">
         <v>0.99936223030090332</v>
       </c>
       <c r="E6" t="s">
-        <v>369</v>
+        <v>985</v>
       </c>
       <c r="F6" s="1">
         <v>102223.13359500001</v>
@@ -1491,14 +3339,14 @@
     <row r="7">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
-        <v>359</v>
+        <v>975</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1">
         <v>0.99965751171112061</v>
       </c>
       <c r="E7" t="s">
-        <v>370</v>
+        <v>986</v>
       </c>
       <c r="F7" s="1">
         <v>134221.16051399999</v>
@@ -1507,14 +3355,14 @@
     <row r="8">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
-        <v>360</v>
+        <v>976</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
         <v>0.99989372491836548</v>
       </c>
       <c r="E8" t="s">
-        <v>371</v>
+        <v>987</v>
       </c>
       <c r="F8" s="1">
         <v>393989.84531999996</v>
@@ -1523,14 +3371,14 @@
     <row r="9">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
-        <v>361</v>
+        <v>977</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1">
         <v>0.99994683265686035</v>
       </c>
       <c r="E9" t="s">
-        <v>372</v>
+        <v>988</v>
       </c>
       <c r="F9" s="1">
         <v>2327811.3491759994</v>
@@ -1547,22 +3395,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>374</v>
+        <v>990</v>
       </c>
       <c r="B1" t="s">
-        <v>375</v>
+        <v>991</v>
       </c>
       <c r="C1" t="s">
-        <v>384</v>
+        <v>1000</v>
       </c>
       <c r="D1" t="s">
-        <v>385</v>
+        <v>1001</v>
       </c>
       <c r="E1" t="s">
-        <v>386</v>
+        <v>1002</v>
       </c>
       <c r="F1" t="s">
-        <v>395</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="2">
@@ -1570,7 +3418,7 @@
         <v>2009</v>
       </c>
       <c r="B2" t="s">
-        <v>376</v>
+        <v>992</v>
       </c>
       <c r="C2" s="1">
         <v>2824.5789878231562</v>
@@ -1579,7 +3427,7 @@
         <v>0.93922626972198486</v>
       </c>
       <c r="E2" t="s">
-        <v>387</v>
+        <v>1003</v>
       </c>
       <c r="F2" s="1">
         <v>7427.2634220259715</v>
@@ -1588,14 +3436,14 @@
     <row r="3">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
-        <v>377</v>
+        <v>993</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1">
         <v>0.96958887577056885</v>
       </c>
       <c r="E3" t="s">
-        <v>388</v>
+        <v>1004</v>
       </c>
       <c r="F3" s="1">
         <v>13488.39384913874</v>
@@ -1604,14 +3452,14 @@
     <row r="4">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
-        <v>378</v>
+        <v>994</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1">
         <v>0.99387890100479126</v>
       </c>
       <c r="E4" t="s">
-        <v>389</v>
+        <v>1005</v>
       </c>
       <c r="F4" s="1">
         <v>38196.156768000001</v>
@@ -1620,14 +3468,14 @@
     <row r="5">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
-        <v>379</v>
+        <v>995</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1">
         <v>0.99691516160964966</v>
       </c>
       <c r="E5" t="s">
-        <v>390</v>
+        <v>1006</v>
       </c>
       <c r="F5" s="1">
         <v>49205.200968000005</v>
@@ -1636,14 +3484,14 @@
     <row r="6">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
-        <v>380</v>
+        <v>996</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1">
         <v>0.99934417009353638</v>
       </c>
       <c r="E6" t="s">
-        <v>391</v>
+        <v>1007</v>
       </c>
       <c r="F6" s="1">
         <v>118355.55177599999</v>
@@ -1652,14 +3500,14 @@
     <row r="7">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
-        <v>381</v>
+        <v>997</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1">
         <v>0.99964779615402222</v>
       </c>
       <c r="E7" t="s">
-        <v>392</v>
+        <v>1008</v>
       </c>
       <c r="F7" s="1">
         <v>158940.49248000002</v>
@@ -1668,14 +3516,14 @@
     <row r="8">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
-        <v>382</v>
+        <v>998</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
         <v>0.99989068508148193</v>
       </c>
       <c r="E8" t="s">
-        <v>393</v>
+        <v>1009</v>
       </c>
       <c r="F8" s="1">
         <v>479378.85349199997</v>
@@ -1684,14 +3532,14 @@
     <row r="9">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
-        <v>383</v>
+        <v>999</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1">
         <v>0.99994534254074097</v>
       </c>
       <c r="E9" t="s">
-        <v>394</v>
+        <v>1010</v>
       </c>
       <c r="F9" s="1">
         <v>3192587.0213159998</v>
@@ -1708,22 +3556,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>396</v>
+        <v>1012</v>
       </c>
       <c r="B1" t="s">
-        <v>397</v>
+        <v>1013</v>
       </c>
       <c r="C1" t="s">
-        <v>406</v>
+        <v>1022</v>
       </c>
       <c r="D1" t="s">
-        <v>407</v>
+        <v>1023</v>
       </c>
       <c r="E1" t="s">
-        <v>408</v>
+        <v>1024</v>
       </c>
       <c r="F1" t="s">
-        <v>417</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="2">
@@ -1731,7 +3579,7 @@
         <v>2010</v>
       </c>
       <c r="B2" t="s">
-        <v>398</v>
+        <v>1014</v>
       </c>
       <c r="C2" s="1">
         <v>3091.1425910001035</v>
@@ -1740,7 +3588,7 @@
         <v>0.938285231590271</v>
       </c>
       <c r="E2" t="s">
-        <v>409</v>
+        <v>1025</v>
       </c>
       <c r="F2" s="1">
         <v>7514.7884521280221</v>
@@ -1749,14 +3597,14 @@
     <row r="3">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
-        <v>399</v>
+        <v>1015</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1">
         <v>0.96911793947219849</v>
       </c>
       <c r="E3" t="s">
-        <v>410</v>
+        <v>1026</v>
       </c>
       <c r="F3" s="1">
         <v>13747.391606108247</v>
@@ -1765,14 +3613,14 @@
     <row r="4">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
-        <v>400</v>
+        <v>1016</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1">
         <v>0.99378412961959839</v>
       </c>
       <c r="E4" t="s">
-        <v>411</v>
+        <v>1027</v>
       </c>
       <c r="F4" s="1">
         <v>38292.759681000003</v>
@@ -1781,14 +3629,14 @@
     <row r="5">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
-        <v>401</v>
+        <v>1017</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1">
         <v>0.99686741828918457</v>
       </c>
       <c r="E5" t="s">
-        <v>412</v>
+        <v>1028</v>
       </c>
       <c r="F5" s="1">
         <v>49642.068630000016</v>
@@ -1797,14 +3645,14 @@
     <row r="6">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
-        <v>402</v>
+        <v>1018</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1">
         <v>0.99933403730392456</v>
       </c>
       <c r="E6" t="s">
-        <v>413</v>
+        <v>1029</v>
       </c>
       <c r="F6" s="1">
         <v>118746.68454000002</v>
@@ -1813,14 +3661,14 @@
     <row r="7">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
-        <v>403</v>
+        <v>1019</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1">
         <v>0.99964231252670288</v>
       </c>
       <c r="E7" t="s">
-        <v>414</v>
+        <v>1030</v>
       </c>
       <c r="F7" s="1">
         <v>148805.54350200001</v>
@@ -1829,14 +3677,14 @@
     <row r="8">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
-        <v>404</v>
+        <v>1020</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
         <v>0.99988901615142822</v>
       </c>
       <c r="E8" t="s">
-        <v>415</v>
+        <v>1031</v>
       </c>
       <c r="F8" s="1">
         <v>398746.96567200008</v>
@@ -1845,14 +3693,14 @@
     <row r="9">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
-        <v>405</v>
+        <v>1021</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1">
         <v>0.99994450807571411</v>
       </c>
       <c r="E9" t="s">
-        <v>416</v>
+        <v>1032</v>
       </c>
       <c r="F9" s="1">
         <v>1848757.1221680001</v>
@@ -1869,22 +3717,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>418</v>
+        <v>1034</v>
       </c>
       <c r="B1" t="s">
-        <v>419</v>
+        <v>1035</v>
       </c>
       <c r="C1" t="s">
-        <v>428</v>
+        <v>1044</v>
       </c>
       <c r="D1" t="s">
-        <v>429</v>
+        <v>1045</v>
       </c>
       <c r="E1" t="s">
-        <v>430</v>
+        <v>1046</v>
       </c>
       <c r="F1" t="s">
-        <v>439</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="2">
@@ -1892,7 +3740,7 @@
         <v>2011</v>
       </c>
       <c r="B2" t="s">
-        <v>420</v>
+        <v>1036</v>
       </c>
       <c r="C2" s="1">
         <v>3542.84912109375</v>
@@ -1901,7 +3749,7 @@
         <v>0.93721121549606323</v>
       </c>
       <c r="E2" t="s">
-        <v>431</v>
+        <v>1047</v>
       </c>
       <c r="F2" s="1">
         <v>10339.130287100314</v>
@@ -1910,14 +3758,14 @@
     <row r="3">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
-        <v>421</v>
+        <v>1037</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1">
         <v>0.96858048439025879</v>
       </c>
       <c r="E3" t="s">
-        <v>432</v>
+        <v>1048</v>
       </c>
       <c r="F3" s="1">
         <v>15366.538025025684</v>
@@ -1926,14 +3774,14 @@
     <row r="4">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
-        <v>422</v>
+        <v>1038</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1">
         <v>0.99367594718933105</v>
       </c>
       <c r="E4" t="s">
-        <v>433</v>
+        <v>1049</v>
       </c>
       <c r="F4" s="1">
         <v>37523.415000000008</v>
@@ -1942,14 +3790,14 @@
     <row r="5">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
-        <v>423</v>
+        <v>1039</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1">
         <v>0.99681288003921509</v>
       </c>
       <c r="E5" t="s">
-        <v>434</v>
+        <v>1050</v>
       </c>
       <c r="F5" s="1">
         <v>45908.899999999994</v>
@@ -1958,14 +3806,14 @@
     <row r="6">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
-        <v>424</v>
+        <v>1040</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1">
         <v>0.99932241439819336</v>
       </c>
       <c r="E6" t="s">
-        <v>435</v>
+        <v>1051</v>
       </c>
       <c r="F6" s="1">
         <v>110935.78200000001</v>
@@ -1974,14 +3822,14 @@
     <row r="7">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
-        <v>425</v>
+        <v>1041</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1">
         <v>0.99963611364364624</v>
       </c>
       <c r="E7" t="s">
-        <v>436</v>
+        <v>1052</v>
       </c>
       <c r="F7" s="1">
         <v>136489.69499999998</v>
@@ -1990,14 +3838,14 @@
     <row r="8">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
-        <v>426</v>
+        <v>1042</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
         <v>0.99988704919815063</v>
       </c>
       <c r="E8" t="s">
-        <v>437</v>
+        <v>1053</v>
       </c>
       <c r="F8" s="1">
         <v>407213.54200000002</v>
@@ -2006,14 +3854,14 @@
     <row r="9">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
-        <v>427</v>
+        <v>1043</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1">
         <v>0.99994355440139771</v>
       </c>
       <c r="E9" t="s">
-        <v>438</v>
+        <v>1054</v>
       </c>
       <c r="F9" s="1">
         <v>2720421.3669999996</v>

</xml_diff>

<commit_message>
last run before october tada delivery
</commit_message>
<xml_diff>
--- a/input_data/admin_data/ECU/_clean/total-pos-ECU.xlsx
+++ b/input_data/admin_data/ECU/_clean/total-pos-ECU.xlsx
@@ -16,7 +16,1063 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="1408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1760" uniqueCount="1760">
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>postax</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
   <si>
     <t>year</t>
   </si>
@@ -4290,22 +5346,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>1320</v>
+        <v>1672</v>
       </c>
       <c r="B1" t="s">
-        <v>1321</v>
+        <v>1673</v>
       </c>
       <c r="C1" t="s">
-        <v>1330</v>
+        <v>1682</v>
       </c>
       <c r="D1" t="s">
-        <v>1331</v>
+        <v>1683</v>
       </c>
       <c r="E1" t="s">
-        <v>1332</v>
+        <v>1684</v>
       </c>
       <c r="F1" t="s">
-        <v>1341</v>
+        <v>1693</v>
       </c>
     </row>
     <row r="2">
@@ -4313,7 +5369,7 @@
         <v>2008</v>
       </c>
       <c r="B2" t="s">
-        <v>1322</v>
+        <v>1674</v>
       </c>
       <c r="C2" s="1">
         <v>2821.7672837582504</v>
@@ -4322,7 +5378,7 @@
         <v>0.94089829921722412</v>
       </c>
       <c r="E2" t="s">
-        <v>1333</v>
+        <v>1685</v>
       </c>
       <c r="F2" s="1">
         <v>6201.1068160713085</v>
@@ -4331,14 +5387,14 @@
     <row r="3">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
-        <v>1323</v>
+        <v>1675</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1">
         <v>0.97042548656463623</v>
       </c>
       <c r="E3" t="s">
-        <v>1334</v>
+        <v>1686</v>
       </c>
       <c r="F3" s="1">
         <v>11701.011533552277</v>
@@ -4347,14 +5403,14 @@
     <row r="4">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
-        <v>1324</v>
+        <v>1676</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1">
         <v>0.99404728412628174</v>
       </c>
       <c r="E4" t="s">
-        <v>1335</v>
+        <v>1687</v>
       </c>
       <c r="F4" s="1">
         <v>34409.242584</v>
@@ -4363,14 +5419,14 @@
     <row r="5">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
-        <v>1325</v>
+        <v>1677</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1">
         <v>0.99700003862380981</v>
       </c>
       <c r="E5" t="s">
-        <v>1336</v>
+        <v>1688</v>
       </c>
       <c r="F5" s="1">
         <v>44915.427675000006</v>
@@ -4379,14 +5435,14 @@
     <row r="6">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
-        <v>1326</v>
+        <v>1678</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1">
         <v>0.99936223030090332</v>
       </c>
       <c r="E6" t="s">
-        <v>1337</v>
+        <v>1689</v>
       </c>
       <c r="F6" s="1">
         <v>102223.13359500001</v>
@@ -4395,14 +5451,14 @@
     <row r="7">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
-        <v>1327</v>
+        <v>1679</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1">
         <v>0.99965751171112061</v>
       </c>
       <c r="E7" t="s">
-        <v>1338</v>
+        <v>1690</v>
       </c>
       <c r="F7" s="1">
         <v>134221.16051399999</v>
@@ -4411,14 +5467,14 @@
     <row r="8">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
-        <v>1328</v>
+        <v>1680</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
         <v>0.99989372491836548</v>
       </c>
       <c r="E8" t="s">
-        <v>1339</v>
+        <v>1691</v>
       </c>
       <c r="F8" s="1">
         <v>393989.84531999996</v>
@@ -4427,14 +5483,14 @@
     <row r="9">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
-        <v>1329</v>
+        <v>1681</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1">
         <v>0.99994683265686035</v>
       </c>
       <c r="E9" t="s">
-        <v>1340</v>
+        <v>1692</v>
       </c>
       <c r="F9" s="1">
         <v>2327811.3491759994</v>
@@ -4451,22 +5507,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>1342</v>
+        <v>1694</v>
       </c>
       <c r="B1" t="s">
-        <v>1343</v>
+        <v>1695</v>
       </c>
       <c r="C1" t="s">
-        <v>1352</v>
+        <v>1704</v>
       </c>
       <c r="D1" t="s">
-        <v>1353</v>
+        <v>1705</v>
       </c>
       <c r="E1" t="s">
-        <v>1354</v>
+        <v>1706</v>
       </c>
       <c r="F1" t="s">
-        <v>1363</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="2">
@@ -4474,7 +5530,7 @@
         <v>2009</v>
       </c>
       <c r="B2" t="s">
-        <v>1344</v>
+        <v>1696</v>
       </c>
       <c r="C2" s="1">
         <v>2824.5789878231562</v>
@@ -4483,7 +5539,7 @@
         <v>0.93922626972198486</v>
       </c>
       <c r="E2" t="s">
-        <v>1355</v>
+        <v>1707</v>
       </c>
       <c r="F2" s="1">
         <v>7427.2634220259715</v>
@@ -4492,14 +5548,14 @@
     <row r="3">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
-        <v>1345</v>
+        <v>1697</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1">
         <v>0.96958887577056885</v>
       </c>
       <c r="E3" t="s">
-        <v>1356</v>
+        <v>1708</v>
       </c>
       <c r="F3" s="1">
         <v>13488.39384913874</v>
@@ -4508,14 +5564,14 @@
     <row r="4">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
-        <v>1346</v>
+        <v>1698</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1">
         <v>0.99387890100479126</v>
       </c>
       <c r="E4" t="s">
-        <v>1357</v>
+        <v>1709</v>
       </c>
       <c r="F4" s="1">
         <v>38196.156768000001</v>
@@ -4524,14 +5580,14 @@
     <row r="5">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
-        <v>1347</v>
+        <v>1699</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1">
         <v>0.99691516160964966</v>
       </c>
       <c r="E5" t="s">
-        <v>1358</v>
+        <v>1710</v>
       </c>
       <c r="F5" s="1">
         <v>49205.200968000005</v>
@@ -4540,14 +5596,14 @@
     <row r="6">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
-        <v>1348</v>
+        <v>1700</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1">
         <v>0.99934417009353638</v>
       </c>
       <c r="E6" t="s">
-        <v>1359</v>
+        <v>1711</v>
       </c>
       <c r="F6" s="1">
         <v>118355.55177599999</v>
@@ -4556,14 +5612,14 @@
     <row r="7">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
-        <v>1349</v>
+        <v>1701</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1">
         <v>0.99964779615402222</v>
       </c>
       <c r="E7" t="s">
-        <v>1360</v>
+        <v>1712</v>
       </c>
       <c r="F7" s="1">
         <v>158940.49248000002</v>
@@ -4572,14 +5628,14 @@
     <row r="8">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
-        <v>1350</v>
+        <v>1702</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
         <v>0.99989068508148193</v>
       </c>
       <c r="E8" t="s">
-        <v>1361</v>
+        <v>1713</v>
       </c>
       <c r="F8" s="1">
         <v>479378.85349199997</v>
@@ -4588,14 +5644,14 @@
     <row r="9">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
-        <v>1351</v>
+        <v>1703</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1">
         <v>0.99994534254074097</v>
       </c>
       <c r="E9" t="s">
-        <v>1362</v>
+        <v>1714</v>
       </c>
       <c r="F9" s="1">
         <v>3192587.0213159998</v>
@@ -4612,22 +5668,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>1364</v>
+        <v>1716</v>
       </c>
       <c r="B1" t="s">
-        <v>1365</v>
+        <v>1717</v>
       </c>
       <c r="C1" t="s">
-        <v>1374</v>
+        <v>1726</v>
       </c>
       <c r="D1" t="s">
-        <v>1375</v>
+        <v>1727</v>
       </c>
       <c r="E1" t="s">
-        <v>1376</v>
+        <v>1728</v>
       </c>
       <c r="F1" t="s">
-        <v>1385</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="2">
@@ -4635,7 +5691,7 @@
         <v>2010</v>
       </c>
       <c r="B2" t="s">
-        <v>1366</v>
+        <v>1718</v>
       </c>
       <c r="C2" s="1">
         <v>3091.1425910001035</v>
@@ -4644,7 +5700,7 @@
         <v>0.938285231590271</v>
       </c>
       <c r="E2" t="s">
-        <v>1377</v>
+        <v>1729</v>
       </c>
       <c r="F2" s="1">
         <v>7514.7884521280221</v>
@@ -4653,14 +5709,14 @@
     <row r="3">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
-        <v>1367</v>
+        <v>1719</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1">
         <v>0.96911793947219849</v>
       </c>
       <c r="E3" t="s">
-        <v>1378</v>
+        <v>1730</v>
       </c>
       <c r="F3" s="1">
         <v>13747.391606108247</v>
@@ -4669,14 +5725,14 @@
     <row r="4">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
-        <v>1368</v>
+        <v>1720</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1">
         <v>0.99378412961959839</v>
       </c>
       <c r="E4" t="s">
-        <v>1379</v>
+        <v>1731</v>
       </c>
       <c r="F4" s="1">
         <v>38292.759681000003</v>
@@ -4685,14 +5741,14 @@
     <row r="5">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
-        <v>1369</v>
+        <v>1721</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1">
         <v>0.99686741828918457</v>
       </c>
       <c r="E5" t="s">
-        <v>1380</v>
+        <v>1732</v>
       </c>
       <c r="F5" s="1">
         <v>49642.068630000016</v>
@@ -4701,14 +5757,14 @@
     <row r="6">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
-        <v>1370</v>
+        <v>1722</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1">
         <v>0.99933403730392456</v>
       </c>
       <c r="E6" t="s">
-        <v>1381</v>
+        <v>1733</v>
       </c>
       <c r="F6" s="1">
         <v>118746.68454000002</v>
@@ -4717,14 +5773,14 @@
     <row r="7">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
-        <v>1371</v>
+        <v>1723</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1">
         <v>0.99964231252670288</v>
       </c>
       <c r="E7" t="s">
-        <v>1382</v>
+        <v>1734</v>
       </c>
       <c r="F7" s="1">
         <v>148805.54350200001</v>
@@ -4733,14 +5789,14 @@
     <row r="8">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
-        <v>1372</v>
+        <v>1724</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
         <v>0.99988901615142822</v>
       </c>
       <c r="E8" t="s">
-        <v>1383</v>
+        <v>1735</v>
       </c>
       <c r="F8" s="1">
         <v>398746.96567200008</v>
@@ -4749,14 +5805,14 @@
     <row r="9">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
-        <v>1373</v>
+        <v>1725</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1">
         <v>0.99994450807571411</v>
       </c>
       <c r="E9" t="s">
-        <v>1384</v>
+        <v>1736</v>
       </c>
       <c r="F9" s="1">
         <v>1848757.1221680001</v>
@@ -4773,22 +5829,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>1386</v>
+        <v>1738</v>
       </c>
       <c r="B1" t="s">
-        <v>1387</v>
+        <v>1739</v>
       </c>
       <c r="C1" t="s">
-        <v>1396</v>
+        <v>1748</v>
       </c>
       <c r="D1" t="s">
-        <v>1397</v>
+        <v>1749</v>
       </c>
       <c r="E1" t="s">
-        <v>1398</v>
+        <v>1750</v>
       </c>
       <c r="F1" t="s">
-        <v>1407</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="2">
@@ -4796,7 +5852,7 @@
         <v>2011</v>
       </c>
       <c r="B2" t="s">
-        <v>1388</v>
+        <v>1740</v>
       </c>
       <c r="C2" s="1">
         <v>3542.84912109375</v>
@@ -4805,7 +5861,7 @@
         <v>0.93721121549606323</v>
       </c>
       <c r="E2" t="s">
-        <v>1399</v>
+        <v>1751</v>
       </c>
       <c r="F2" s="1">
         <v>10339.130287100314</v>
@@ -4814,14 +5870,14 @@
     <row r="3">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
-        <v>1389</v>
+        <v>1741</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1">
         <v>0.96858048439025879</v>
       </c>
       <c r="E3" t="s">
-        <v>1400</v>
+        <v>1752</v>
       </c>
       <c r="F3" s="1">
         <v>15366.538025025684</v>
@@ -4830,14 +5886,14 @@
     <row r="4">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
-        <v>1390</v>
+        <v>1742</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1">
         <v>0.99367594718933105</v>
       </c>
       <c r="E4" t="s">
-        <v>1401</v>
+        <v>1753</v>
       </c>
       <c r="F4" s="1">
         <v>37523.415000000008</v>
@@ -4846,14 +5902,14 @@
     <row r="5">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
-        <v>1391</v>
+        <v>1743</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1">
         <v>0.99681288003921509</v>
       </c>
       <c r="E5" t="s">
-        <v>1402</v>
+        <v>1754</v>
       </c>
       <c r="F5" s="1">
         <v>45908.899999999994</v>
@@ -4862,14 +5918,14 @@
     <row r="6">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
-        <v>1392</v>
+        <v>1744</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1">
         <v>0.99932241439819336</v>
       </c>
       <c r="E6" t="s">
-        <v>1403</v>
+        <v>1755</v>
       </c>
       <c r="F6" s="1">
         <v>110935.78200000001</v>
@@ -4878,14 +5934,14 @@
     <row r="7">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
-        <v>1393</v>
+        <v>1745</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1">
         <v>0.99963611364364624</v>
       </c>
       <c r="E7" t="s">
-        <v>1404</v>
+        <v>1756</v>
       </c>
       <c r="F7" s="1">
         <v>136489.69499999998</v>
@@ -4894,14 +5950,14 @@
     <row r="8">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
-        <v>1394</v>
+        <v>1746</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
         <v>0.99988704919815063</v>
       </c>
       <c r="E8" t="s">
-        <v>1405</v>
+        <v>1757</v>
       </c>
       <c r="F8" s="1">
         <v>407213.54200000002</v>
@@ -4910,14 +5966,14 @@
     <row r="9">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
-        <v>1395</v>
+        <v>1747</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1">
         <v>0.99994355440139771</v>
       </c>
       <c r="E9" t="s">
-        <v>1406</v>
+        <v>1758</v>
       </c>
       <c r="F9" s="1">
         <v>2720421.3669999996</v>

</xml_diff>